<commit_message>
john rahm won the masters and I fixed the elasticNet naming issue
</commit_message>
<xml_diff>
--- a/results/ElasticNet.xlsx
+++ b/results/ElasticNet.xlsx
@@ -495,26 +495,23 @@
         <is>
           <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector',
-                 &lt;__main__.NamedFeatureSelector object at 0x7f91c7468640&gt;),
+                 SelectFromModel(estimator=ExtraTreesClassifier(random_state=42))),
                 ('model',
-                 AdaBoostClassifier(estimator=LogisticRegression(l1_ratio=0.1,
-                                                                 max_iter=1000,
-                                                                 penalty='elasticnet',
-                                                                 random_state=42,
-                                                                 solver='saga'),
-                                    n_estimators=10, random_state=42))])</t>
+                 LogisticRegression(l1_ratio=0.7, max_iter=1000,
+                                    penalty='elasticnet', random_state=42,
+                                    solver='saga'))])</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7058823529411764</v>
+        <v>0.675</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f91244bc250&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 10, 'model__estimator__solver': 'saga', 'model__estimator__penalty': 'elasticnet', 'model__estimator__l1_ratio': 0.1, 'model__estimator__class_weight': None}</t>
+          <t>{'selector': SelectFromModel(estimator=ExtraTreesClassifier(random_state=42)), 'scaler': MinMaxScaler(), 'model__solver': 'saga', 'model__penalty': 'elasticnet', 'model__l1_ratio': 0.7, 'model__class_weight': None}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -523,44 +520,43 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[1 1 1 1 1 1 1 1 1 1 1 1]</t>
+          <t>[1 1 1 1 1 1 0 0 1 0 0 1]</t>
         </is>
       </c>
       <c r="G2" t="n">
         <v>42</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6403210023268138</v>
+        <v>0.7226190422428765</v>
       </c>
       <c r="I2" t="n">
-        <v>0.09259510926561515</v>
+        <v>0.02060886693193312</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5771007038712921</v>
+        <v>0.5708267950731186</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1212835179341145</v>
+        <v>0.1195666986043687</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()), ('selector', None),
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+                ('selector',
+                 &lt;__main__.NamedFeatureSelector object at 0x7f84bc13a220&gt;),
                 ('model',
-                 AdaBoostClassifier(estimator=LogisticRegression(l1_ratio=0.01,
-                                                                 max_iter=1000,
-                                                                 penalty='elasticnet',
-                                                                 random_state=42,
-                                                                 solver='saga'),
-                                    random_state=42))])</t>
+                 LogisticRegression(l1_ratio=0.95, max_iter=1000,
+                                    penalty='elasticnet', random_state=42,
+                                    solver='saga'))])</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7102941176470587</v>
+        <v>0.7058823529411764</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'selector': None, 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__solver': 'saga', 'model__estimator__penalty': 'elasticnet', 'model__estimator__l1_ratio': 0.01, 'model__estimator__class_weight': None}</t>
+          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f84bc13a280&gt;, 'scaler': MinMaxScaler(), 'model__solver': 'saga', 'model__penalty': 'elasticnet', 'model__l1_ratio': 0.95, 'model__class_weight': None}</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -580,92 +576,85 @@
         <v>69</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6200692750874723</v>
+        <v>0.7206601951574058</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1276651807959677</v>
+        <v>0.01863472491005711</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5840976552858905</v>
+        <v>0.6459373316634346</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1453575871855953</v>
+        <v>0.1097797140122413</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector',
-                 SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1',
-                                                     random_state=42))),
-                ('model',
-                 AdaBoostClassifier(estimator=LogisticRegression(l1_ratio=0.001,
-                                                                 max_iter=1000,
-                                                                 penalty='elasticnet',
-                                                                 random_state=42,
-                                                                 solver='saga'),
-                                    random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7186624649859944</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'selector': SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1', random_state=42)), 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__solver': 'saga', 'model__estimator__penalty': 'elasticnet', 'model__estimator__l1_ratio': 0.001, 'model__estimator__class_weight': None}</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.7777777777777777</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[0 1 0 0 1 1 1 1 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[1 1 1 1 1 1 0 1 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>23</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.5565892096759216</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.1238284137601524</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.5276599165540342</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1306490699870561</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
         <is>
           <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector',
                  SelectFromModel(estimator=ExtraTreesClassifier(random_state=42))),
                 ('model',
-                 AdaBoostClassifier(estimator=LogisticRegression(l1_ratio=0.001,
-                                                                 max_iter=1000,
-                                                                 penalty='elasticnet',
-                                                                 random_state=42,
-                                                                 solver='saga'),
-                                    random_state=42))])</t>
+                 LogisticRegression(l1_ratio=0.7, max_iter=1000,
+                                    penalty='elasticnet', random_state=42,
+                                    solver='saga'))])</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.7296078431372548</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'selector': SelectFromModel(estimator=ExtraTreesClassifier(random_state=42)), 'scaler': MinMaxScaler(), 'model__solver': 'saga', 'model__penalty': 'elasticnet', 'model__l1_ratio': 0.7, 'model__class_weight': None}</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.7777777777777777</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[0 1 0 0 1 1 1 1 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[1 1 1 1 1 1 0 1 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>23</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.7176654084892338</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.02092927649931291</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.6611737738024502</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.08846323748931456</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+                ('selector',
+                 SelectFromModel(estimator=ExtraTreesClassifier(random_state=42))),
+                ('model',
+                 LogisticRegression(l1_ratio=0.3, max_iter=1000,
+                                    penalty='elasticnet', random_state=42,
+                                    solver='saga'))])</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7839379084967321</v>
+        <v>0.7841830065359476</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'selector': SelectFromModel(estimator=ExtraTreesClassifier(random_state=42)), 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__solver': 'saga', 'model__estimator__penalty': 'elasticnet', 'model__estimator__l1_ratio': 0.001, 'model__estimator__class_weight': None}</t>
+          <t>{'selector': SelectFromModel(estimator=ExtraTreesClassifier(random_state=42)), 'scaler': MinMaxScaler(), 'model__solver': 'saga', 'model__penalty': 'elasticnet', 'model__l1_ratio': 0.3, 'model__class_weight': None}</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -685,16 +674,16 @@
         <v>99</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6874354218330191</v>
+        <v>0.7314862579019984</v>
       </c>
       <c r="I5" t="n">
-        <v>0.08586573297021793</v>
+        <v>0.01586547553482015</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6928471606824548</v>
+        <v>0.7022387103637104</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1079292773490324</v>
+        <v>0.08565157848675527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>